<commit_message>
1 新增表情资源 2 修改SceneType.Demo为Client
</commit_message>
<xml_diff>
--- a/Excel/#ConstValue.xlsx
+++ b/Excel/#ConstValue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17680"/>
+    <workbookView windowHeight="17775"/>
   </bookViews>
   <sheets>
     <sheet name="ConstValue" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>#</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>聊天系统消息uid</t>
+  </si>
+  <si>
+    <t>ChatGetCount</t>
+  </si>
+  <si>
+    <t>聊天消息单次拉取数量</t>
   </si>
 </sst>
 </file>
@@ -1076,20 +1082,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C2:F8"/>
+  <dimension ref="C2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" outlineLevelRow="7" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="21.1272727272727" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7545454545455" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.2636363636364" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.5545454545455" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.1727272727273" style="3" customWidth="1"/>
-    <col min="6" max="6" width="53.5363636363636" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7583333333333" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.2666666666667" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.5583333333333" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.175" style="3" customWidth="1"/>
+    <col min="6" max="6" width="53.5333333333333" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1098,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="13.5" spans="3:6">
+    <row r="3" spans="3:6">
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="13.5" spans="3:6">
+    <row r="4" spans="3:6">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1124,7 +1130,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" ht="13.5" spans="3:6">
+    <row r="5" spans="3:6">
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1168,14 +1174,28 @@
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>12</v>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>